<commit_message>
update import, export excel, export pdf
</commit_message>
<xml_diff>
--- a/PWLPOS.v2/public/template_data/barang.xlsx
+++ b/PWLPOS.v2/public/template_data/barang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Tugas-WebLanjut\Minggu-8\Jobsheet8\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Tugas-WebLanjut\PWLPOS.v2\public\template_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495F2588-545B-412E-8BCE-C8DF8FAF4F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0023A63-50EC-40EF-8AA3-0672D26BF212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A34A5B1E-EE70-4D4B-9F9D-5963B13C0A86}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>kategori_id</t>
   </si>
@@ -51,34 +51,16 @@
     <t>harga_jual</t>
   </si>
   <si>
-    <t>BRG0012</t>
-  </si>
-  <si>
-    <t>BRG0013</t>
-  </si>
-  <si>
-    <t>BRG0014</t>
-  </si>
-  <si>
-    <t>BRG0015</t>
-  </si>
-  <si>
-    <t>BRG0016</t>
-  </si>
-  <si>
-    <t>Sweater</t>
-  </si>
-  <si>
-    <t>Spidol</t>
-  </si>
-  <si>
-    <t>The Gelas</t>
-  </si>
-  <si>
-    <t>Roti Boy</t>
-  </si>
-  <si>
-    <t>Kulkas</t>
+    <t>BRG0017</t>
+  </si>
+  <si>
+    <t>Kaos oblong</t>
+  </si>
+  <si>
+    <t>BRG0018</t>
+  </si>
+  <si>
+    <t>Celana Pendek</t>
   </si>
 </sst>
 </file>
@@ -448,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4EDA28-8793-475C-A3E1-E46CE82E69D7}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,81 +470,30 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
-        <v>80000</v>
+        <v>40000</v>
       </c>
       <c r="E2" s="2">
-        <v>100000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="2">
-        <v>5000</v>
+        <v>50000</v>
       </c>
       <c r="E3" s="2">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1500</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2500</v>
-      </c>
-      <c r="E5" s="2">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2">
-        <v>400000</v>
-      </c>
-      <c r="E6" s="2">
-        <v>500000</v>
+        <v>75000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>